<commit_message>
removed 2 lines from normal remotes
</commit_message>
<xml_diff>
--- a/ac translations/Chinese.xlsx
+++ b/ac translations/Chinese.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\programming\Remote - Projects\helper projects\Remotes App Translation Project\ac translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zvi\Desktop\dev\helpers\translation fetcher\ac translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="Chinese Translation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1208,6 +1208,27 @@
     <t>没有连接 \ 等待互联网...</t>
   </si>
   <si>
+    <t>你好 :) \ 为你加载一些东西...</t>
+  </si>
+  <si>
+    <t>振动 :(</t>
+  </si>
+  <si>
+    <t>我的公司不在这里 :(</t>
+  </si>
+  <si>
+    <t>否 :(</t>
+  </si>
+  <si>
+    <t>我的遥控器丢失了 :(</t>
+  </si>
+  <si>
+    <t>我的电视不在这里 :(</t>
+  </si>
+  <si>
+    <t>空调遥控 ____  - 现在免费</t>
+  </si>
+  <si>
     <t>限时免费版
 遥控空调失去了你的空调？没问题！
 **免责声明
@@ -1218,8 +1239,6 @@
 不知道这是什么意思？你可以尝试下载应用程序，看看它是否工作
 你的遥控器丢失了？只要问我们从应用程序
 特征：
-*从手机上控制你的____电视机
-*音量控制你的电视（上/下/静音/ AV）
 *保存您最喜爱的遥控器，方便使用
 *没有安装，只需点击和播放
 *令人惊叹的设计与凉爽和简单的界面
@@ -1227,32 +1246,11 @@
 请随时与我们联系
 电视遥控器为您的点击播放机顶盒</t>
   </si>
-  <si>
-    <t>你好 :) \ 为你加载一些东西...</t>
-  </si>
-  <si>
-    <t>振动 :(</t>
-  </si>
-  <si>
-    <t>我的公司不在这里 :(</t>
-  </si>
-  <si>
-    <t>否 :(</t>
-  </si>
-  <si>
-    <t>我的遥控器丢失了 :(</t>
-  </si>
-  <si>
-    <t>我的电视不在这里 :(</t>
-  </si>
-  <si>
-    <t>空调遥控 ____  - 现在免费</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12">
     <font>
       <sz val="12"/>
@@ -1735,11 +1733,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -1784,7 +1782,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -2196,7 +2194,7 @@
         <v>74</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F38" t="s">
         <v>75</v>
@@ -2292,7 +2290,7 @@
         <v>89</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F46" t="s">
         <v>90</v>
@@ -2426,7 +2424,7 @@
         <v>111</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F57" t="s">
         <v>112</v>
@@ -2594,7 +2592,7 @@
         <v>137</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F71" t="s">
         <v>138</v>
@@ -3026,7 +3024,7 @@
         <v>207</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F107" t="s">
         <v>208</v>
@@ -3038,7 +3036,7 @@
         <v>209</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F108" t="s">
         <v>210</v>
@@ -3170,7 +3168,7 @@
         <v>89</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F119" t="s">
         <v>231</v>
@@ -3368,7 +3366,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="363" thickBot="1">
+    <row r="136" spans="1:6" ht="345.75" thickBot="1">
       <c r="A136" s="8" t="s">
         <v>263</v>
       </c>
@@ -3376,7 +3374,7 @@
         <v>268</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="F136" t="s">
         <v>264</v>

</xml_diff>